<commit_message>
Computed all scores based on deployed models
</commit_message>
<xml_diff>
--- a/hypertuning_results_wordsonly.xlsx
+++ b/hypertuning_results_wordsonly.xlsx
@@ -55,16 +55,16 @@
     <t>n_accuracy</t>
   </si>
   <si>
-    <t>0:05:23</t>
-  </si>
-  <si>
-    <t>0:46:49</t>
-  </si>
-  <si>
-    <t>0:07:18</t>
-  </si>
-  <si>
-    <t>0:25:04</t>
+    <t>0:00:02</t>
+  </si>
+  <si>
+    <t>0:08:41</t>
+  </si>
+  <si>
+    <t>0:01:08</t>
+  </si>
+  <si>
+    <t>0:00:07</t>
   </si>
 </sst>
 </file>
@@ -467,28 +467,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>9000</v>
+        <v>5000</v>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1491</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>60.57142857142858</v>
+        <v>92.0952380952381</v>
       </c>
       <c r="G2" t="n">
-        <v>182558</v>
+        <v>105000</v>
       </c>
       <c r="H2" t="n">
-        <v>146046</v>
+        <v>84000</v>
       </c>
       <c r="I2" t="n">
-        <v>36512</v>
+        <v>21000</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
@@ -503,7 +503,7 @@
         <v>13</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6420628834355828</v>
+        <v>0.969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>